<commit_message>
Correção das tabelas e adição do relatório em reports
</commit_message>
<xml_diff>
--- a/references/DESCRIÇÃO DOS DATASETS - CIENCIA DOS DADOS.xlsx
+++ b/references/DESCRIÇÃO DOS DATASETS - CIENCIA DOS DADOS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Desktop\ARQUIVOS PC ANTIGO\PLANOS DE AULA E LIVROS FACULDADE\CIENCIA DOS DADOS\ds_project\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFA7BAE-8F1D-4D06-B9EA-9DC6A001F90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40388F00-DBDB-418A-A8E0-FD61A2F4CFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-732" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-732" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATASET PLAYSTATION" sheetId="1" r:id="rId1"/>
@@ -1128,8 +1128,8 @@
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="42.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1447,11 +1447,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1460,7 +1460,7 @@
     <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1704,12 +1704,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="4:4" ht="15.75" customHeight="1">
-      <c r="D18" s="49"/>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1721,10 +1717,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1732,8 +1728,8 @@
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2057,8 +2053,12 @@
         <v>11</v>
       </c>
     </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+      <c r="C22" s="49"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>